<commit_message>
correcion de vuneberalidad de accesos para usuarios, definicion de permisos para usuarios dependiendo de su rol y cambios en los zerializer aplicando el camelCase
</commit_message>
<xml_diff>
--- a/frontAgrosis/public/plantillas/plantillaUsuarios.xlsx
+++ b/frontAgrosis/public/plantillas/plantillaUsuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\OneDrive\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2E584F2-FAF6-47C8-A147-3E15258382FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28339942-3C4F-4175-B012-E693031C91F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{90D229D2-A9F0-49EF-BC1A-9272E041ADD0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>identificacion</t>
   </si>
@@ -42,19 +42,10 @@
     <t>email</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>nombre</t>
   </si>
   <si>
     <t>apellido</t>
-  </si>
-  <si>
-    <t>rol</t>
-  </si>
-  <si>
-    <t>ficha</t>
   </si>
 </sst>
 </file>
@@ -94,15 +85,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -110,12 +107,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -123,16 +135,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -448,73 +467,343 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2227941-3DF2-444A-A9FA-5782F5070D65}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="J5" s="6"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="6"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="6"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="6"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="6"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="6"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="6"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="6"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="6"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="6"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="6"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="6"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="6"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="6"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="6"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="6"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="6"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="6"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="6"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="6"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="6"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="6"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="6"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="6"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="6"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>